<commit_message>
update of new version of Lecture 8 & 9 (add paragraphs)
</commit_message>
<xml_diff>
--- a/files/QT/Lecture_8_data.xlsx
+++ b/files/QT/Lecture_8_data.xlsx
@@ -917,25 +917,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>129.2213754300486</c:v>
+                  <c:v>81.22137543004855</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1966.592539697031</c:v>
+                  <c:v>1990.592539697031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3839.745442516999</c:v>
+                  <c:v>3724.745442516999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9087.323037596655</c:v>
+                  <c:v>9052.323037596655</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12766.79658812509</c:v>
+                  <c:v>12542.79658812509</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16677.71427517355</c:v>
+                  <c:v>15633.71427517355</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22078.79931067171</c:v>
+                  <c:v>22117.79931067171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H14" s="9">
         <f ca="1">$F$10*F14^2+RANDBETWEEN(-F14/2,F14/2)</f>
-        <v>129.22137543004857</v>
+        <v>81.221375430048553</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="H15" s="9">
         <f t="shared" ref="H15:H20" ca="1" si="2">$F$10*F15^2+RANDBETWEEN(-F15/2,F15/2)</f>
-        <v>1966.5925396970308</v>
+        <v>1990.5925396970308</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="H16" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3839.7454425169985</v>
+        <v>3724.7454425169985</v>
       </c>
     </row>
     <row r="17" spans="2:8">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="H17" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>9087.3230375966559</v>
+        <v>9052.3230375966559</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="H18" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>12766.796588125095</v>
+        <v>12542.796588125095</v>
       </c>
     </row>
     <row r="19" spans="2:8">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="H19" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>16677.714275173552</v>
+        <v>15633.714275173552</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="H20" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>22078.799310671708</v>
+        <v>22117.799310671708</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with question in class
</commit_message>
<xml_diff>
--- a/files/QT/Lecture_8_data.xlsx
+++ b/files/QT/Lecture_8_data.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="section 1" sheetId="2" r:id="rId1"/>
     <sheet name="section 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="17">
   <si>
     <t>&amp;</t>
   </si>
@@ -48,12 +49,39 @@
   <si>
     <t>\\</t>
   </si>
+  <si>
+    <t>Absolute Deviation</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>With Lecture's formula</t>
+  </si>
+  <si>
+    <t>With Excel Direct Formula</t>
+  </si>
+  <si>
+    <t>|x_i-\bar(x)|</t>
+  </si>
+  <si>
+    <t>(X_i-\bar(X))^2</t>
+  </si>
+  <si>
+    <t>X_i</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +116,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -115,7 +151,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -155,8 +191,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,8 +225,24 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -202,6 +262,10 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -221,6 +285,10 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,11 +458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2117224760"/>
-        <c:axId val="2117219896"/>
+        <c:axId val="2109287432"/>
+        <c:axId val="2109292392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2117224760"/>
+        <c:axId val="2109287432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,12 +491,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117219896"/>
+        <c:crossAx val="2109292392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2117219896"/>
+        <c:axId val="2109292392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -462,7 +530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117224760"/>
+        <c:crossAx val="2109287432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -754,11 +822,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2117171672"/>
-        <c:axId val="2117168776"/>
+        <c:axId val="2109391384"/>
+        <c:axId val="2109394296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2117171672"/>
+        <c:axId val="2109391384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,12 +836,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117168776"/>
+        <c:crossAx val="2109394296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2117168776"/>
+        <c:axId val="2109394296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117171672"/>
+        <c:crossAx val="2109391384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -917,25 +985,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>81.22137543004855</c:v>
+                  <c:v>121.2213754300486</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1990.592539697031</c:v>
+                  <c:v>1860.592539697031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3724.745442516999</c:v>
+                  <c:v>3816.745442516999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9052.323037596655</c:v>
+                  <c:v>8259.323037596655</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12542.79658812509</c:v>
+                  <c:v>13368.79658812509</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15633.71427517355</c:v>
+                  <c:v>16115.71427517355</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22117.79931067171</c:v>
+                  <c:v>20826.79931067171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,11 +1018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2117139672"/>
-        <c:axId val="2117136776"/>
+        <c:axId val="2109423496"/>
+        <c:axId val="2109426392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2117139672"/>
+        <c:axId val="2109423496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,12 +1032,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117136776"/>
+        <c:crossAx val="2109426392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2117136776"/>
+        <c:axId val="2109426392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +1047,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117139672"/>
+        <c:crossAx val="2109423496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1426,7 +1494,7 @@
   <dimension ref="B1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1735,7 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -2065,7 +2133,7 @@
       </c>
       <c r="H14" s="9">
         <f ca="1">$F$10*F14^2+RANDBETWEEN(-F14/2,F14/2)</f>
-        <v>81.221375430048553</v>
+        <v>121.22137543004855</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -2086,7 +2154,7 @@
       </c>
       <c r="H15" s="9">
         <f t="shared" ref="H15:H20" ca="1" si="2">$F$10*F15^2+RANDBETWEEN(-F15/2,F15/2)</f>
-        <v>1990.5925396970308</v>
+        <v>1860.5925396970308</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -2107,7 +2175,7 @@
       </c>
       <c r="H16" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3724.7454425169985</v>
+        <v>3816.7454425169985</v>
       </c>
     </row>
     <row r="17" spans="2:8">
@@ -2128,7 +2196,7 @@
       </c>
       <c r="H17" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>9052.3230375966559</v>
+        <v>8259.3230375966559</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -2149,7 +2217,7 @@
       </c>
       <c r="H18" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>12542.796588125095</v>
+        <v>13368.796588125095</v>
       </c>
     </row>
     <row r="19" spans="2:8">
@@ -2170,7 +2238,7 @@
       </c>
       <c r="H19" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>15633.714275173552</v>
+        <v>16115.714275173552</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -2191,7 +2259,7 @@
       </c>
       <c r="H20" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>22117.799310671708</v>
+        <v>20826.799310671708</v>
       </c>
     </row>
   </sheetData>
@@ -2203,4 +2271,251 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <f>(B3-$B$17)^2</f>
+        <v>19.506944444444446</v>
+      </c>
+      <c r="D3" s="14">
+        <f>ABS(B3-$B$17)</f>
+        <v>4.416666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="14">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7">
+        <f>(B4-$B$17)^2</f>
+        <v>11.673611111111112</v>
+      </c>
+      <c r="D4" s="14">
+        <f>ABS(B4-$B$17)</f>
+        <v>3.416666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <f>(B5-$B$17)^2</f>
+        <v>11.673611111111112</v>
+      </c>
+      <c r="D5" s="14">
+        <f>ABS(B5-$B$17)</f>
+        <v>3.416666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="14">
+        <v>5</v>
+      </c>
+      <c r="C6" s="7">
+        <f>(B6-$B$17)^2</f>
+        <v>2.0069444444444451</v>
+      </c>
+      <c r="D6" s="14">
+        <f>ABS(B6-$B$17)</f>
+        <v>1.416666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="14">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <f>(B7-$B$17)^2</f>
+        <v>0.17361111111111135</v>
+      </c>
+      <c r="D7" s="14">
+        <f>ABS(B7-$B$17)</f>
+        <v>0.41666666666666696</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="14">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7">
+        <f>(B8-$B$17)^2</f>
+        <v>0.34027777777777746</v>
+      </c>
+      <c r="D8" s="14">
+        <f>ABS(B8-$B$17)</f>
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="14">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <f>(B9-$B$17)^2</f>
+        <v>0.34027777777777746</v>
+      </c>
+      <c r="D9" s="14">
+        <f>ABS(B9-$B$17)</f>
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="14">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <f>(B10-$B$17)^2</f>
+        <v>2.5069444444444433</v>
+      </c>
+      <c r="D10" s="14">
+        <f>ABS(B10-$B$17)</f>
+        <v>1.583333333333333</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="14">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7">
+        <f>(B11-$B$17)^2</f>
+        <v>2.5069444444444433</v>
+      </c>
+      <c r="D11" s="14">
+        <f>ABS(B11-$B$17)</f>
+        <v>1.583333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="14">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7">
+        <f>(B12-$B$17)^2</f>
+        <v>6.6736111111111098</v>
+      </c>
+      <c r="D12" s="14">
+        <f>ABS(B12-$B$17)</f>
+        <v>2.583333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="14">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7">
+        <f>(B13-$B$17)^2</f>
+        <v>6.6736111111111098</v>
+      </c>
+      <c r="D13" s="14">
+        <f>ABS(B13-$B$17)</f>
+        <v>2.583333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="14">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7">
+        <f>(B14-$B$17)^2</f>
+        <v>12.840277777777775</v>
+      </c>
+      <c r="D14" s="14">
+        <f>ABS(B14-$B$17)</f>
+        <v>3.583333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="30">
+      <c r="B16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7">
+        <f>AVERAGE(B3:B14)</f>
+        <v>6.416666666666667</v>
+      </c>
+      <c r="C17" s="7">
+        <f>1/12*SUM(B3:B14)</f>
+        <v>6.4166666666666661</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="11">
+        <f>MEDIAN(B3:B14)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="7">
+        <f>STDEVP(B3:B14)</f>
+        <v>2.5317429218272185</v>
+      </c>
+      <c r="C19" s="7">
+        <f>SQRT(1/12*SUM(C3:C14))</f>
+        <v>2.5317429218272185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="7">
+        <f>AVEDEV(B3:B14)</f>
+        <v>2.1805555555555549</v>
+      </c>
+      <c r="C20" s="7">
+        <f>1/12*SUM(D3:D14)</f>
+        <v>2.1805555555555549</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>